<commit_message>
Code updated 23-01-15 11:30:35
</commit_message>
<xml_diff>
--- a/Season_Trophies/81.xlsx
+++ b/Season_Trophies/81.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -396,7 +396,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18612</t>
+          <t>20274</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -416,24 +416,24 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>4589</t>
+          <t>4604</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1115</t>
+          <t>4979</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>26424998</t>
+          <t>1820342</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"煙神在此 爾等跪拜 ᶻᵍˣ"</t>
+          <t>摸鱼者三战</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -443,24 +443,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>6625</t>
+          <t>6101</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2798</t>
+          <t>2035</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>26588375</t>
+          <t>1951758</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>kusipao</t>
+          <t>我來找你了</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -470,24 +470,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>6211</t>
+          <t>6583</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>7796</t>
+          <t>3334</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>31217211</t>
+          <t>3477306</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>解憂雜貨鋪㊥</t>
+          <t>"MeGa Tsai"</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -497,24 +497,24 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>5508</t>
+          <t>6330</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>293</t>
+          <t>3396</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6940556</t>
+          <t>3946814</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
+          <t>"小瑩 潘"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -524,24 +524,24 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>6995</t>
+          <t>6320</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>372</t>
+          <t>7369</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>31267627</t>
+          <t>4229136</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>"㊥ Martin"</t>
+          <t>"totoro wu"</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -551,24 +551,24 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>6948</t>
+          <t>5732</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>447</t>
+          <t>4868</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>8741713</t>
+          <t>5691528</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">㊥大咖玩家ky </t>
+          <t>ABearBear</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -578,24 +578,24 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>6905</t>
+          <t>6111</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>539</t>
+          <t>41011</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>32613475</t>
+          <t>6016757</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"李 无 善 德"</t>
+          <t>Xx邪罗罗xX</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -605,24 +605,24 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>6855</t>
+          <t>3534</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1153</t>
+          <t>7349</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>29211638</t>
+          <t>6510348</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"㊥ PhononDisperse"</t>
+          <t>Bonpoisson</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -632,24 +632,24 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>6614</t>
+          <t>5738</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>3648</t>
+          <t>424</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>21665473</t>
+          <t>6940556</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"Dog Gamedesiger"</t>
+          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -659,24 +659,24 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>7186</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>5210</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>20199374</t>
+          <t>7025661</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>RuanFan</t>
+          <t>"F ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -686,24 +686,24 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>6845</t>
+          <t>6075</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1486</t>
+          <t>54417</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11783968</t>
+          <t>7587898</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>F---119</t>
+          <t>藍精靈ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -713,24 +713,24 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>6508</t>
+          <t>2970</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1752</t>
+          <t>285</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>27468237</t>
+          <t>8741713</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>佛系复仇者秀川</t>
+          <t xml:space="preserve">㊥大咖玩家ky </t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -740,24 +740,24 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>6434</t>
+          <t>7281</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1790</t>
+          <t>4899</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1951758</t>
+          <t>9541747</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>我來找你了</t>
+          <t>豹子头林冲</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -767,24 +767,24 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>6423</t>
+          <t>6108</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2298</t>
+          <t>1220</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3946814</t>
+          <t>11783968</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>"小瑩 潘"</t>
+          <t>F---119</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -794,24 +794,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>6305</t>
+          <t>6840</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2328</t>
+          <t>8012</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>25376635</t>
+          <t>14424176</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>"sanchez ᶻᵍˣ"</t>
+          <t>天才少年老纪</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -821,24 +821,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>6299</t>
+          <t>5630</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2585</t>
+          <t>3216</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>21345373</t>
+          <t>16206490</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>林北不講武德</t>
+          <t>㊥Godcys</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -848,24 +848,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>6248</t>
+          <t>6351</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2892</t>
+          <t>524</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>46422609</t>
+          <t>20199374</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>㊥林天大大神</t>
+          <t>RuanFan</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -875,24 +875,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>6194</t>
+          <t>7137</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2980</t>
+          <t>6531</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3477306</t>
+          <t>20737010</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"MeGa Tsai"</t>
+          <t>混着玩...</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -902,24 +902,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>6179</t>
+          <t>5881</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3226</t>
+          <t>2303</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16206490</t>
+          <t>21345373</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>㊥Godcys</t>
+          <t>林北不講武德</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -929,24 +929,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>6525</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>3678</t>
+          <t>4191</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>7025661</t>
+          <t>21665473</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>"F ᶻᵍˣ"</t>
+          <t>"Dog Gamedesiger"</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -956,24 +956,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>6071</t>
+          <t>6196</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>3915</t>
+          <t>6768</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>26280580</t>
+          <t>21735478</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>꧁S.TIGRESS꧂ᶻᵍˣ</t>
+          <t>耀翔fly</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -983,24 +983,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>6036</t>
+          <t>5834</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4092</t>
+          <t>72376</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>24733875</t>
+          <t>23687250</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Kikkik</t>
+          <t>"jetlijp ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1010,24 +1010,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>6012</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4602</t>
+          <t>3692</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>33656016</t>
+          <t>24733875</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>㊥☆梅海听雪☆</t>
+          <t>Kikkik</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1037,24 +1037,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>5941</t>
+          <t>6268</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4785</t>
+          <t>2430</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>49553719</t>
+          <t>25376635</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>"Oreo Captain Sir"</t>
+          <t>"sanchez ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1064,24 +1064,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>5919</t>
+          <t>6492</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4894</t>
+          <t>2769</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>9541747</t>
+          <t>26280580</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>豹子头林冲</t>
+          <t>꧁S.TIGRESS꧂ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1091,24 +1091,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>5905</t>
+          <t>6426</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5056</t>
+          <t>983</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>47758619</t>
+          <t>26424998</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>"㊥ Moon ㊥"</t>
+          <t>"煙神在此 爾等跪拜 ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1118,24 +1118,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>6924</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5091</t>
+          <t>4273</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>30411791</t>
+          <t>26588375</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
+          <t>kusipao</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1145,24 +1145,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>6182</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5573</t>
+          <t>2994</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>44955827</t>
+          <t>27468237</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>丶小阿狸丿</t>
+          <t>佛系复仇者秀川</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1172,24 +1172,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>5823</t>
+          <t>6388</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>465</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5691528</t>
+          <t>27484940</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ABearBear</t>
+          <t>"Zephyr ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1199,24 +1199,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>5746</t>
+          <t>7167</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>6776</t>
+          <t>38845</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>21735478</t>
+          <t>28387448</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>"fly kao"</t>
+          <t>☜⊙‖⊙☞</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>3632</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>6822</t>
+          <t>1880</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>43800641</t>
+          <t>29211638</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>㊥蛋蛋大</t>
+          <t>"㊥ PhononDisperse"</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1253,24 +1253,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>5649</t>
+          <t>6623</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>7678</t>
+          <t>7894</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>6510348</t>
+          <t>29729468</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Bonpoisson</t>
+          <t>"风神舞动 WDᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1280,24 +1280,24 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>5523</t>
+          <t>5648</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>8105</t>
+          <t>12555</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>29729468</t>
+          <t>29861826</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>"风神舞动 WDᶻᵍˣ"</t>
+          <t>★★★Eric★★★</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1307,24 +1307,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>5468</t>
+          <t>5194</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>8793</t>
+          <t>55810</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>14424176</t>
+          <t>30129740</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>天才少年老纪</t>
+          <t>JohnyWS</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1334,24 +1334,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>5382</t>
+          <t>2915</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>13193</t>
+          <t>4173</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>29861826</t>
+          <t>30411791</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>★★★Eric★★★</t>
+          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1361,24 +1361,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>4985</t>
+          <t>6198</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>37435</t>
+          <t>7608</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>28387448</t>
+          <t>31217211</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>☜⊙‖⊙☞</t>
+          <t>解憂雜貨鋪㊥</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1388,24 +1388,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>3632</t>
+          <t>5695</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>49908</t>
+          <t>471</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>35384730</t>
+          <t>31267627</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>"king of war £"</t>
+          <t>"㊥ Martin"</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1415,24 +1415,24 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>3116</t>
+          <t>7164</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>53436</t>
+          <t>4466</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7587898</t>
+          <t>32478707</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>藍精靈ᶻᵍˣ</t>
+          <t>"Bt So"</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1442,24 +1442,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2970</t>
+          <t>6157</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>71509</t>
+          <t>520</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>23687250</t>
+          <t>32613475</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>"jetlijp ᶻᵍˣ"</t>
+          <t>"李 无 善 德"</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1469,24 +1469,24 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>7138</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>99046</t>
+          <t>5754</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>57484853</t>
+          <t>33656016</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>"vector to islam"</t>
+          <t>㊥☆梅海听雪☆</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1496,267 +1496,267 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2009</t>
+          <t>6021</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>21862</t>
+          <t>49144</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>37861953</t>
+          <t>35384730</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>"Durex ๑• . •๑"</t>
+          <t>"king of war £"</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>4413</t>
+          <t>3205</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>19362</t>
+          <t>6894</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>38809086</t>
+          <t>43800641</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Kouenᶻᵍˣ</t>
+          <t>㊥蛋蛋大</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>4548</t>
+          <t>5813</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6033</t>
+          <t>4111</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>38711610</t>
+          <t>44955827</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>"心灵有为 1"</t>
+          <t>丶小阿狸丿</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>5760</t>
+          <t>6207</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6387</t>
+          <t>10530</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>28749280</t>
+          <t>45967307</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>㊥老船⛵⛵</t>
+          <t>Ricky</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>5713</t>
+          <t>5351</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6890</t>
+          <t>3122</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>43812707</t>
+          <t>46422609</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>bbtt</t>
+          <t>㊥林天大大神</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>5638</t>
+          <t>6366</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>7739</t>
+          <t>4509</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>13738844</t>
+          <t>47758619</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>"Chen Hao"</t>
+          <t>"㊥ Moon ㊥"</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>5516</t>
+          <t>6152</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>13014</t>
+          <t>5504</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>53060417</t>
+          <t>49553719</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>㊥老纳信耶稣</t>
+          <t>"Oreo Captain Sir"</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>4999</t>
+          <t>6046</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>15377</t>
+          <t>18691</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>53520939</t>
+          <t>54189845</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>㊥虎哥tiger</t>
+          <t>"going down ®"</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>4798</t>
+          <t>4684</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>18836</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>31495601</t>
+          <t>57484853</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>陈晓军</t>
+          <t>"vector to islam"</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>4577</t>
+          <t>1997</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>30310</t>
+          <t>54618</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>55769051</t>
+          <t>29565</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>㊥叮叮当.</t>
+          <t>"aK.j Zhong ㊥"</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1766,24 +1766,24 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>3943</t>
+          <t>2962</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>38311</t>
+          <t>44737</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>45070827</t>
+          <t>68132</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>㊥山东老灶丿</t>
+          <t>"㊖TW9 百媚生"</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1793,24 +1793,24 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>3591</t>
+          <t>3380</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>4333</t>
+          <t>27658</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1820342</t>
+          <t>1550355</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>摸鱼者三战</t>
+          <t>"皓茵 世界"</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1820,24 +1820,24 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>5981</t>
+          <t>4150</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>7667</t>
+          <t>7057</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>12639656</t>
+          <t>4493731</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>"wu huang"</t>
+          <t>Player-1527362</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1847,24 +1847,24 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>5525</t>
+          <t>5784</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>7850</t>
+          <t>21025</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>4493731</t>
+          <t>4756174</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Player-1527362</t>
+          <t>純希です</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1874,24 +1874,24 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>5501</t>
+          <t>4567</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>9830</t>
+          <t>19494</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>47131129</t>
+          <t>6809364</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>NAM</t>
+          <t>"Scorp IP"</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1901,24 +1901,24 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>5277</t>
+          <t>4640</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>10666</t>
+          <t>10360</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>22885399</t>
+          <t>7852598</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>余文琪</t>
+          <t>seiji</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1928,24 +1928,24 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>5201</t>
+          <t>5366</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>11809</t>
+          <t>17129</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7852598</t>
+          <t>8057001</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>seiji</t>
+          <t>㊥兵者诡道也</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1955,14 +1955,14 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>5100</t>
+          <t>4781</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>11841</t>
+          <t>11028</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>5098</t>
+          <t>5311</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>12817</t>
+          <t>7359</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>42434117</t>
+          <t>12639656</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>㊥有双飞鸟</t>
+          <t>"wu huang"</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,24 +2009,24 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>5016</t>
+          <t>5735</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>14056</t>
+          <t>7428</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>56133764</t>
+          <t>13738844</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>ustcarter</t>
+          <t>"Chen Hao"</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2036,24 +2036,24 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>4906</t>
+          <t>5722</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>14219</t>
+          <t>32761</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>49710892</t>
+          <t>14110169</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>MMMMMMM</t>
+          <t>"Pasiony CANQ"</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2063,24 +2063,24 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>4893</t>
+          <t>3910</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>15977</t>
+          <t>42232</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>25435189</t>
+          <t>22161051</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Jose</t>
+          <t>Botz5</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2090,24 +2090,24 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>4752</t>
+          <t>3481</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>16363</t>
+          <t>10959</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>54698813</t>
+          <t>22885399</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>閃亮唐老鴨</t>
+          <t>余文琪</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2117,24 +2117,24 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>4725</t>
+          <t>5316</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>17916</t>
+          <t>17046</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>54915122</t>
+          <t>25435189</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>平胸救世界</t>
+          <t>Jose</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>4627</t>
+          <t>4787</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>19178</t>
+          <t>6983</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8057001</t>
+          <t>28749280</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>㊥兵者诡道也</t>
+          <t>㊥老船⛵⛵</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2171,24 +2171,24 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>4558</t>
+          <t>5795</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>19694</t>
+          <t>19000</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>6809364</t>
+          <t>31495601</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>"Scorp IP"</t>
+          <t>陈晓军</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2198,24 +2198,24 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>4531</t>
+          <t>4666</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>21731</t>
+          <t>21345</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>4756174</t>
+          <t>32316256</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>純希です</t>
+          <t>"秋の風 .."</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2225,24 +2225,24 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>4419</t>
+          <t>4553</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>24849</t>
+          <t>22823</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>38561634</t>
+          <t>37861953</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>"Ambrose PT"</t>
+          <t>"Durex ๑• . •๑"</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2252,24 +2252,24 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>4230</t>
+          <t>4475</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>25984</t>
+          <t>25043</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>32316256</t>
+          <t>38561634</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>"秋の風 .."</t>
+          <t>"Ambrose PT"</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2279,24 +2279,24 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>4161</t>
+          <t>4311</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>27644</t>
+          <t>5950</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>1550355</t>
+          <t>38711610</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>"皓茵 世界"</t>
+          <t>"心灵有为 1"</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2306,24 +2306,24 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>4070</t>
+          <t>6001</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>28475</t>
+          <t>19776</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>38893233</t>
+          <t>38809086</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>"快乐 二哈"</t>
+          <t>Kouenᶻᵍˣ</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2333,24 +2333,24 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>4030</t>
+          <t>4628</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>30988</t>
+          <t>22387</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>14110169</t>
+          <t>38893233</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>"Pasiony CANQ"</t>
+          <t>"快乐 二哈"</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2360,14 +2360,14 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>3910</t>
+          <t>4508</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>31170</t>
+          <t>31645</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2387,24 +2387,24 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>3902</t>
+          <t>3959</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>33192</t>
+          <t>13559</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>47146736</t>
+          <t>42434117</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>"HK 品瑜"</t>
+          <t>㊥有双飞鸟</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2414,24 +2414,24 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>3817</t>
+          <t>5084</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>36328</t>
+          <t>7178</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>55860890</t>
+          <t>43812707</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>㊥Ethan</t>
+          <t>bbtt</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2441,24 +2441,24 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>3681</t>
+          <t>5763</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>39729</t>
+          <t>38496</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>56573048</t>
+          <t>45070827</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Xiaotian</t>
+          <t>㊥山东老灶丿</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2468,24 +2468,24 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>3531</t>
+          <t>3648</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>44296</t>
+          <t>10090</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>22161051</t>
+          <t>47131129</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Botz5</t>
+          <t>NAM</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2495,24 +2495,24 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>3345</t>
+          <t>5392</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>44828</t>
+          <t>21538</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>68132</t>
+          <t>47146736</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>"㊖TW9 百媚生"</t>
+          <t>"HK 品瑜"</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2522,24 +2522,24 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>3322</t>
+          <t>4545</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>51693</t>
+          <t>13976</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>56500325</t>
+          <t>49710892</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>haruharuyukizg9735</t>
+          <t>MMMMMMM</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2549,24 +2549,24 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>3042</t>
+          <t>5042</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>53656</t>
+          <t>11960</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>29565</t>
+          <t>53060417</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>"aK.j Zhong ㊥"</t>
+          <t>㊥老纳信耶稣</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2576,24 +2576,24 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2962</t>
+          <t>5240</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>93167</t>
+          <t>15232</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>57837683</t>
+          <t>53520939</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>我的世界只有你</t>
+          <t>㊥虎哥tiger</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2603,240 +2603,240 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>4926</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>8877</t>
+          <t>15112</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>44378757</t>
+          <t>54698813</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
+          <t>閃亮唐老鴨</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>5371</t>
+          <t>4938</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>27895</t>
+          <t>17132</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>44708798</t>
+          <t>54915122</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>"㊥ mythgod"</t>
+          <t>平胸救世界</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>4058</t>
+          <t>4781</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>46689</t>
+          <t>31018</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>54588689</t>
+          <t>55769051</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>㊥墨衍枫迹☜</t>
+          <t>㊥叮叮当.</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>3249</t>
+          <t>3987</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>5000</t>
+          <t>33682</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>7857221</t>
+          <t>55860890</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Rename</t>
+          <t>㊥Ethan</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>5893</t>
+          <t>3873</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>8310</t>
+          <t>12260</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>4229136</t>
+          <t>56133764</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>"totoro wu"</t>
+          <t>ustcarter</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>5441</t>
+          <t>5219</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>17194</t>
+          <t>51526</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>56500325</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>haruharuyukizg9735</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>4673</t>
+          <t>3096</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>18481</t>
+          <t>40758</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>25163202</t>
+          <t>56573048</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>"sam yang"</t>
+          <t>Xiaotian</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>3545</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>25597</t>
+          <t>93490</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>25479797</t>
+          <t>57837683</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>"Mohamed Alnaqbi"</t>
+          <t>我的世界只有你</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>4185</t>
+          <t>2121</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>28006</t>
+          <t>57695</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>1222440</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>"Sneaky Ninja Panda"</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2846,24 +2846,24 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>4052</t>
+          <t>2845</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>29689</t>
+          <t>48591</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>37069173</t>
+          <t>3391765</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>詹toniii</t>
+          <t>马er</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2873,24 +2873,24 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>3974</t>
+          <t>3228</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>29381</t>
+          <t>75014</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>5367482</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>Ігор</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2900,24 +2900,24 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>3987</t>
+          <t>2459</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>30104</t>
+          <t>5428</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>28855852</t>
+          <t>7857221</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>tiger</t>
+          <t>Rename</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2927,24 +2927,24 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>3952</t>
+          <t>6055</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>33347</t>
+          <t>63090</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>9718882</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>小霸王2021</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2954,24 +2954,24 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>3811</t>
+          <t>2681</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>33602</t>
+          <t>44682</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>51841127</t>
+          <t>11645391</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>"Muhammad Shox"</t>
+          <t>"omar omar"</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2981,24 +2981,24 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>3801</t>
+          <t>3383</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>34157</t>
+          <t>39181</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>18082891</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3008,24 +3008,24 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>3776</t>
+          <t>3616</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>33923</t>
+          <t>20050</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>25163202</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>"sam yang"</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3035,24 +3035,24 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>3787</t>
+          <t>4614</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>34892</t>
+          <t>26837</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>25479797</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>"Mohamed Alnaqbi"</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3062,24 +3062,24 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>3745</t>
+          <t>4197</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>37610</t>
+          <t>30580</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>46289694</t>
+          <t>28855852</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>㊥Vincent</t>
+          <t>tiger</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3089,24 +3089,24 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>3623</t>
+          <t>4006</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>37811</t>
+          <t>18919</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>31134300</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>McMaX</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3116,24 +3116,24 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>3615</t>
+          <t>4671</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>43346</t>
+          <t>29874</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>37069173</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>詹toniii</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3143,24 +3143,24 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>3384</t>
+          <t>4038</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>44562</t>
+          <t>53460</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>56732705</t>
+          <t>38994054</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>时间温柔皆遗憾</t>
+          <t>chengnan</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3170,24 +3170,24 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>3333</t>
+          <t>3011</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>44744</t>
+          <t>7503</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>44378757</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Globalking</t>
+          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3197,24 +3197,24 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>3326</t>
+          <t>5710</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>44779</t>
+          <t>28150</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>18082891</t>
+          <t>44708798</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>"㊥ mythgod"</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3224,24 +3224,24 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>3325</t>
+          <t>4124</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>44808</t>
+          <t>38060</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>46289694</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>㊥Vincent</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3251,24 +3251,24 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>3323</t>
+          <t>3670</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>47555</t>
+          <t>57118</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>47227626</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>Player-47227626</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3278,24 +3278,24 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>3217</t>
+          <t>2865</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>51904</t>
+          <t>29363</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>55499394</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Player-55499394</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3305,24 +3305,24 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>3034</t>
+          <t>4064</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>52270</t>
+          <t>37595</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>38994054</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>chengnan</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3332,24 +3332,24 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>3020</t>
+          <t>3693</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>55394</t>
+          <t>30760</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>48634530</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>leezhenrui</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3359,24 +3359,24 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>2896</t>
+          <t>3998</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>56337</t>
+          <t>34858</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>1222440</t>
+          <t>51841127</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>"Sneaky Ninja Panda"</t>
+          <t>"Muhammad Shox"</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3386,14 +3386,14 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>2860</t>
+          <t>3825</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>57764</t>
+          <t>59052</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3413,24 +3413,24 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>2812</t>
+          <t>2800</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>58169</t>
+          <t>54842</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>47227626</t>
+          <t>52997727</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Player-47227626</t>
+          <t>larios</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3440,24 +3440,24 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>2800</t>
+          <t>2953</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>60101</t>
+          <t>35214</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>55810157</t>
+          <t>54085771</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Beard</t>
+          <t>㊥Matthieu</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3467,24 +3467,24 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>2740</t>
+          <t>3810</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>60801</t>
+          <t>46065</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>58203298</t>
+          <t>54588689</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>AdyYouTubeSs</t>
+          <t>㊥墨衍枫迹☜</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3494,24 +3494,24 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>2720</t>
+          <t>3325</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>62124</t>
+          <t>35915</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>9718882</t>
+          <t>54778421</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>小霸王2021</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3521,24 +3521,24 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>2683</t>
+          <t>3776</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>64913</t>
+          <t>53368</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>58340439</t>
+          <t>55499394</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Player-58340439</t>
+          <t>Player-55499394</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3548,24 +3548,24 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>2614</t>
+          <t>3014</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>73926</t>
+          <t>34606</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>5367482</t>
+          <t>55634661</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Ігор</t>
+          <t>Opalus</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3575,24 +3575,24 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>2464</t>
+          <t>3836</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>83910</t>
+          <t>58358</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>57556179</t>
+          <t>55810157</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>特战新生代英雄</t>
+          <t>Beard</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3602,213 +3602,213 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>2254</t>
+          <t>2823</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>58805</t>
+          <t>43081</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>41849539</t>
+          <t>56379103</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>三号馆馆主</t>
+          <t>Globalking</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>2780</t>
+          <t>3446</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>31906</t>
+          <t>44569</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>56585361</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>"㊥ go策划我要ali"</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>3873</t>
+          <t>3386</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>54150</t>
+          <t>32416</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>56700848</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>工口漫画老师</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>2942</t>
+          <t>3923</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>485</t>
+          <t>43125</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>27484940</t>
+          <t>56732705</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>"Zephyr ᶻᵍˣ"</t>
+          <t>时间温柔皆遗憾</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>6886</t>
+          <t>3444</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>3872</t>
+          <t>85321</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>32478707</t>
+          <t>57556179</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>"Bt So"</t>
+          <t>特战新生代英雄</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>6041</t>
+          <t>2247</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>6734</t>
+          <t>60972</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>22497</t>
+          <t>58203298</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>xixihahagggᶻᵍˣ</t>
+          <t>AdyYouTubeSs</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>5662</t>
+          <t>2741</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>6776</t>
+          <t>64818</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>20737010</t>
+          <t>58340439</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>混着玩...</t>
+          <t>Player-58340439</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>2637</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10257</t>
+          <t>5822</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>45967307</t>
+          <t>22497</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Ricky</t>
+          <t>xixihahagggᶻᵍˣ</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3818,24 +3818,24 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>5236</t>
+          <t>6015</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>51302</t>
+          <t>70042</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>55210350</t>
+          <t>41463618</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>一个过客而已</t>
+          <t>qi ye</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -3845,24 +3845,24 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>3057</t>
+          <t>2534</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>58825</t>
+          <t>58437</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>57038133</t>
+          <t>41849539</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Player-57038133</t>
+          <t>三号馆馆主</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3872,24 +3872,24 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>2779</t>
+          <t>2820</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>61027</t>
+          <t>64031</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>57219176</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>青莲道人</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3899,24 +3899,24 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>2714</t>
+          <t>2657</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>64722</t>
+          <t>31493</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -3926,24 +3926,24 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>2619</t>
+          <t>3966</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>68732</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>41463618</t>
+          <t>51816877</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>qi ye</t>
+          <t>且行且珍惜</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3953,24 +3953,24 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>2542</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>73182</t>
+          <t>52742</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>57722377</t>
+          <t>55210350</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>VI空白IV</t>
+          <t>一个过客而已</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3980,24 +3980,24 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>2476</t>
+          <t>3040</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>87954</t>
+          <t>56128</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>57905163</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>ABC—57905163</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4007,24 +4007,24 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>2193</t>
+          <t>2901</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>90168</t>
+          <t>62067</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>58463042</t>
+          <t>57219176</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>DiamondSloth80</t>
+          <t>青莲道人</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4034,24 +4034,24 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>2162</t>
+          <t>2711</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>93985</t>
+          <t>73051</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>57867293</t>
+          <t>57722377</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Player-57867293</t>
+          <t>VI空白IV</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4061,14 +4061,14 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>2087</t>
+          <t>2492</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>104007</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -4095,17 +4095,17 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>108806</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>58526469</t>
+          <t>57809206</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>ItaloFlausino</t>
+          <t>"king 1"</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4115,24 +4115,24 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>1772</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>109026</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>58537218</t>
+          <t>57847993</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>"BRAWL TALK"</t>
+          <t>龘梦心裘千仞</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4142,24 +4142,24 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>1767</t>
+          <t>1508</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>114029</t>
+          <t>91159</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>58415620</t>
+          <t>57867293</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>"el pepe"</t>
+          <t>Player-57867293</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4169,24 +4169,24 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>1685</t>
+          <t>2164</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>115990</t>
+          <t>89342</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>58437456</t>
+          <t>57905163</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>中国人不骗中国人</t>
+          <t>ABC—57905163</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4196,24 +4196,24 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>1654</t>
+          <t>2190</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>118592</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>58380905</t>
+          <t>57908454</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Player-58380905</t>
+          <t>Player-57908454</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4223,14 +4223,14 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>1622</t>
+          <t>1100</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>127329</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -4257,17 +4257,17 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>130556</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>57847993</t>
+          <t>58368224</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>龘梦心裘千仞</t>
+          <t>战争雷霆杯</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4277,24 +4277,24 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>1508</t>
+          <t>1400</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>144809</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>58425274</t>
+          <t>58380905</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Player-58425274</t>
+          <t>Player-58380905</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4304,24 +4304,24 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>1411</t>
+          <t>1648</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>146394</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>58368224</t>
+          <t>58386875</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>战争雷霆杯</t>
+          <t>ExquisiteAgreement33</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4331,24 +4331,24 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>1400</t>
+          <t>1328</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>154771</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>58415620</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>"el pepe"</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4358,24 +4358,24 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>1346</t>
+          <t>1685</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>157228</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>58386875</t>
+          <t>58425274</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>ExquisiteAgreement33</t>
+          <t>Player-58425274</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -4385,24 +4385,24 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>1328</t>
+          <t>1411</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>169813</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>58494374</t>
+          <t>58437456</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Kirinfire</t>
+          <t>中国人不骗中国人</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -4412,14 +4412,14 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>1259</t>
+          <t>1639</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>190237</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4446,17 +4446,17 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>197953</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>57908454</t>
+          <t>58494374</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Player-57908454</t>
+          <t>Kirinfire</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -4466,24 +4466,24 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>1259</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>51816877</t>
+          <t>58526469</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>且行且珍惜</t>
+          <t>ItaloFlausino</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -4493,24 +4493,24 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1781</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>57809206</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>"king 1"</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -4520,51 +4520,51 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1346</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>51858</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>41848598</t>
+          <t>58584744</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>国家一级保护沙雕</t>
+          <t>ronaldo</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>3036</t>
+          <t>1198</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>3469</t>
+          <t>10575</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>9913517</t>
+          <t>6010122</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>"Kenny Chan"</t>
+          <t>"Edward Peng"</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -4574,24 +4574,24 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>6104</t>
+          <t>5347</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>9327</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>6010122</t>
+          <t>8850180</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>"Edward Peng"</t>
+          <t>30624300</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -4601,24 +4601,24 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>5321</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>57119</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>15755724</t>
+          <t>9195340</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>"Last Good"</t>
+          <t>Namllllllik</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -4628,24 +4628,24 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>2833</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>4025</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>12648101</t>
+          <t>9913517</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>"player 198827"</t>
+          <t>"Kenny Chan"</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -4655,24 +4655,24 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6220</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>9195340</t>
+          <t>12648101</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Namllllllik</t>
+          <t>"player 198827"</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -4689,17 +4689,17 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>57473</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>8850180</t>
+          <t>15755724</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>30624300</t>
+          <t>"Last Good"</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -4709,14 +4709,14 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2853</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4737,6 +4737,33 @@
       <c r="E162" t="inlineStr">
         <is>
           <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>52177</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>41848598</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>国家一级保护沙雕</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>3065</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-24 11:31:58
</commit_message>
<xml_diff>
--- a/Season_Trophies/81.xlsx
+++ b/Season_Trophies/81.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1746,17 +1746,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>54618</t>
+          <t>7268</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>29565</t>
+          <t>48293354</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>"aK.j Zhong ㊥"</t>
+          <t>"Goodbye ‏ᴠᴇᴄ"</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1766,24 +1766,24 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2962</t>
+          <t>4826</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>44737</t>
+          <t>1719</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>68132</t>
+          <t>39287605</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>"㊖TW9 百媚生"</t>
+          <t>"VEC milespapa"</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1793,24 +1793,24 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>3380</t>
+          <t>5499</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>27658</t>
+          <t>1974</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1550355</t>
+          <t>24262874</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>"皓茵 世界"</t>
+          <t>Dogeball</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1820,24 +1820,24 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>4150</t>
+          <t>5449</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>7057</t>
+          <t>2373</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>4493731</t>
+          <t>6179013</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Player-1527362</t>
+          <t>"ｍｒ.  ｓｔｉｇｍａｔｉｚｅｄ"</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1847,24 +1847,24 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>5784</t>
+          <t>5377</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>21025</t>
+          <t>2421</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>4756174</t>
+          <t>32004387</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>純希です</t>
+          <t>Crickrat2357</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1874,24 +1874,24 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>4567</t>
+          <t>5370</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>19494</t>
+          <t>2866</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>6809364</t>
+          <t>1803405</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>"Scorp IP"</t>
+          <t>"Smiler ᵛᵉᶜ"</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1901,24 +1901,24 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>4640</t>
+          <t>5301</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>10360</t>
+          <t>3497</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7852598</t>
+          <t>42396645</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>seiji</t>
+          <t>"Fran64 ∆π"</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1928,24 +1928,24 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>5366</t>
+          <t>5216</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>17129</t>
+          <t>3772</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8057001</t>
+          <t>48929103</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>㊥兵者诡道也</t>
+          <t>Monkeyᵛᵉᶜ</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1955,24 +1955,24 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>4781</t>
+          <t>5180</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>11028</t>
+          <t>4347</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>11582001</t>
+          <t>41975808</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>iMinatoX4</t>
+          <t>Christian</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>5311</t>
+          <t>5116</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7359</t>
+          <t>4527</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>12639656</t>
+          <t>38465364</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>"wu huang"</t>
+          <t>Rocking-RobinVEC</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,24 +2009,24 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>5735</t>
+          <t>5098</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7428</t>
+          <t>4768</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>13738844</t>
+          <t>51180802</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>"Chen Hao"</t>
+          <t>"Go Noles VEC"</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2036,24 +2036,24 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>5722</t>
+          <t>5072</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>32761</t>
+          <t>5297</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>14110169</t>
+          <t>32330920</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>"Pasiony CANQ"</t>
+          <t>"Los Lobos ᴹʸᴬ"</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2063,24 +2063,24 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>3910</t>
+          <t>5020</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>42232</t>
+          <t>5364</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>22161051</t>
+          <t>29562912</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Botz5</t>
+          <t>"RockingRobin VEC"</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2090,24 +2090,24 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>3481</t>
+          <t>5013</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>10959</t>
+          <t>6393</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>22885399</t>
+          <t>31206030</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>余文琪</t>
+          <t>"VEC Jenny"</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2117,24 +2117,24 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>5316</t>
+          <t>4913</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>17046</t>
+          <t>6615</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>25435189</t>
+          <t>30801950</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Jose</t>
+          <t>"Hobbes VEC"</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>4787</t>
+          <t>4891</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6983</t>
+          <t>6778</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>28749280</t>
+          <t>46690829</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>㊥老船⛵⛵</t>
+          <t>macPSU</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2171,24 +2171,24 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>5795</t>
+          <t>4873</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>19000</t>
+          <t>7574</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>31495601</t>
+          <t>2429559</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>陈晓军</t>
+          <t>"Torgon ɔǝʌ"</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2198,24 +2198,24 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>4666</t>
+          <t>4799</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>21345</t>
+          <t>7606</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>32316256</t>
+          <t>49819488</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>"秋の風 .."</t>
+          <t>Myst</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2225,24 +2225,24 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>4553</t>
+          <t>4795</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>22823</t>
+          <t>7884</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>37861953</t>
+          <t>32536732</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>"Durex ๑• . •๑"</t>
+          <t>"its iggy"</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2252,24 +2252,24 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>4475</t>
+          <t>4769</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>25043</t>
+          <t>8115</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>38561634</t>
+          <t>51279372</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>"Ambrose PT"</t>
+          <t>"PeZxH4 ＶＥＣ"</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2279,24 +2279,24 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>4311</t>
+          <t>4745</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>5950</t>
+          <t>8175</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>38711610</t>
+          <t>8686641</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>心灵有为</t>
+          <t>"NIKĀ IS BACK ″"</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2306,24 +2306,24 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>6001</t>
+          <t>4739</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>19776</t>
+          <t>8319</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>38809086</t>
+          <t>4831713</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Kouenᶻᵍˣ</t>
+          <t>"RAJA N"</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2333,24 +2333,24 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>4628</t>
+          <t>4727</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>22387</t>
+          <t>8364</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>38893233</t>
+          <t>47490553</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>"快乐 二哈"</t>
+          <t>"VEC SneakySnake"</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2360,24 +2360,24 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>4508</t>
+          <t>4723</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>31645</t>
+          <t>8378</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>38995116</t>
+          <t>2917344</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>"Ramesh Pavai Nam"</t>
+          <t>"Forrest Hump34"</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2387,24 +2387,24 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>3959</t>
+          <t>4722</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>13559</t>
+          <t>8430</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>42434117</t>
+          <t>47933909</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>㊥有双飞鸟</t>
+          <t>AllahsMineswpⱤØ₣</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2414,24 +2414,24 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>5084</t>
+          <t>4717</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7178</t>
+          <t>8620</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>43812707</t>
+          <t>46956348</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>bbtt</t>
+          <t>rckaiser</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2441,24 +2441,24 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>5763</t>
+          <t>4703</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>38496</t>
+          <t>8811</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>45070827</t>
+          <t>33592072</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>㊥山东老灶丿</t>
+          <t>"VEC Y"</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2468,24 +2468,24 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>3648</t>
+          <t>4688</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>10090</t>
+          <t>8808</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>47131129</t>
+          <t>55119285</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>NAM</t>
+          <t>Chi</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2495,24 +2495,24 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>5392</t>
+          <t>4688</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>21538</t>
+          <t>9090</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>47146736</t>
+          <t>21518036</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>"HK 品瑜"</t>
+          <t>"El Que ɔǝʌ"</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2522,24 +2522,24 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>4545</t>
+          <t>4663</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>13976</t>
+          <t>9138</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>49710892</t>
+          <t>40926559</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>MMMMMMM</t>
+          <t>"Mark ᵛᵉᶜ"</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2549,24 +2549,24 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>5042</t>
+          <t>4659</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>11960</t>
+          <t>9282</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>53060417</t>
+          <t>38934511</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>㊥老纳信耶稣</t>
+          <t>"DetroitKid33 ᵥₑc"</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2576,24 +2576,24 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>5240</t>
+          <t>4647</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>15232</t>
+          <t>10206</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>53520939</t>
+          <t>49036101</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>㊥虎哥tiger</t>
+          <t>"Ace Minaka"</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2603,24 +2603,24 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>4926</t>
+          <t>4579</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>15112</t>
+          <t>10329</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>54698813</t>
+          <t>40995501</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>閃亮唐老鴨</t>
+          <t>Confirm</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2630,24 +2630,24 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>4938</t>
+          <t>4569</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>17132</t>
+          <t>10356</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>54915122</t>
+          <t>48569177</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>平胸救世界</t>
+          <t>Tardnugget</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2657,24 +2657,24 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>4781</t>
+          <t>4567</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>31018</t>
+          <t>10470</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>55769051</t>
+          <t>20724497</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>㊥叮叮当.</t>
+          <t>"Keith Klein"</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2684,24 +2684,24 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>3987</t>
+          <t>4558</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>33682</t>
+          <t>11387</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>55860890</t>
+          <t>9455119</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>㊥Ethan</t>
+          <t>Randy</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2711,24 +2711,24 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>3873</t>
+          <t>4493</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>12260</t>
+          <t>12003</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>56133764</t>
+          <t>45989212</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>ustcarter</t>
+          <t>xEvan</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2738,24 +2738,24 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>5219</t>
+          <t>4452</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>51526</t>
+          <t>13922</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>56500325</t>
+          <t>7443176</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>haruharuyukizg9735</t>
+          <t>AloNio42</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2765,24 +2765,24 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>3096</t>
+          <t>4322</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>40758</t>
+          <t>14043</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>56573048</t>
+          <t>23930021</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Xiaotian</t>
+          <t>Scrubber</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2792,24 +2792,24 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>3545</t>
+          <t>4314</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>93490</t>
+          <t>14093</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>57837683</t>
+          <t>52401413</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>我的世界只有你</t>
+          <t>"VEC HAKUREI"</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2819,105 +2819,105 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>2121</t>
+          <t>4310</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>57695</t>
+          <t>23436</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>1222440</t>
+          <t>47156718</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>"Sneaky Ninja Panda"</t>
+          <t>OoOoO</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>2845</t>
+          <t>3828</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>48591</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>3747329</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>"Fix the game"</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>3228</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>75014</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>5367482</t>
+          <t>31275569</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Ігор</t>
+          <t>Grim_</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>2459</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>5428</t>
+          <t>57695</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>7857221</t>
+          <t>1222440</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Disparaître</t>
+          <t>"Sneaky Ninja Panda"</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2927,24 +2927,24 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>6055</t>
+          <t>2845</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>63090</t>
+          <t>48591</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>9718882</t>
+          <t>3391765</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>小霸王2021</t>
+          <t>马er</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2954,24 +2954,24 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>2681</t>
+          <t>3228</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>44682</t>
+          <t>75014</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>5367482</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>Ігор</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2981,24 +2981,24 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>3383</t>
+          <t>2459</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>39181</t>
+          <t>5428</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>18082891</t>
+          <t>7857221</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Disparaître</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3008,24 +3008,24 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>3616</t>
+          <t>6055</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>20050</t>
+          <t>63090</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>25163202</t>
+          <t>9718882</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>"sam yang"</t>
+          <t>小霸王2021</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3035,24 +3035,24 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>4614</t>
+          <t>2681</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>26837</t>
+          <t>44682</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>25479797</t>
+          <t>11645391</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>"Mohamed Alnaqbi"</t>
+          <t>"omar omar"</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3062,24 +3062,24 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>4197</t>
+          <t>3383</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>30580</t>
+          <t>39181</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>28855852</t>
+          <t>18082891</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>tiger</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3089,24 +3089,24 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>4006</t>
+          <t>3616</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>18919</t>
+          <t>20050</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>25163202</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>"sam yang"</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3116,24 +3116,24 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>4671</t>
+          <t>4614</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>29874</t>
+          <t>26837</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>37069173</t>
+          <t>25479797</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>詹toniii</t>
+          <t>"Mohamed Alnaqbi"</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3143,24 +3143,24 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>4038</t>
+          <t>4197</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>53460</t>
+          <t>30580</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>38994054</t>
+          <t>28855852</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>chengnan</t>
+          <t>tiger</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3170,24 +3170,24 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>3011</t>
+          <t>4006</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>7503</t>
+          <t>18919</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>44378757</t>
+          <t>31134300</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
+          <t>McMaX</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3197,24 +3197,24 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>5710</t>
+          <t>4671</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>28150</t>
+          <t>29874</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>44708798</t>
+          <t>37069173</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>"㊥ mythgod"</t>
+          <t>詹toniii</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3224,24 +3224,24 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>4124</t>
+          <t>4038</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>38060</t>
+          <t>53460</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>46289694</t>
+          <t>38994054</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>㊥Vincent</t>
+          <t>chengnan</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3251,24 +3251,24 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>3670</t>
+          <t>3011</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>57118</t>
+          <t>7503</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>47227626</t>
+          <t>44378757</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Player-47227626</t>
+          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3278,24 +3278,24 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>2865</t>
+          <t>5710</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>29363</t>
+          <t>28150</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>44708798</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>"㊥ mythgod"</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3305,24 +3305,24 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>4064</t>
+          <t>4124</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>37595</t>
+          <t>38060</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>46289694</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>㊥Vincent</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3332,24 +3332,24 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>3693</t>
+          <t>3670</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>30760</t>
+          <t>57118</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>47227626</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>Player-47227626</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3359,24 +3359,24 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>3998</t>
+          <t>2865</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>34858</t>
+          <t>29363</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>51841127</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>"Muhammad Shox"</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3386,24 +3386,24 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>3825</t>
+          <t>4064</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>59052</t>
+          <t>37595</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>52792063</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>"Tramaine Dowlen"</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3413,24 +3413,24 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>2800</t>
+          <t>3693</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>54842</t>
+          <t>30760</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>48634530</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>leezhenrui</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3440,24 +3440,24 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>2953</t>
+          <t>3998</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>35214</t>
+          <t>34858</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>51841127</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>"Muhammad Shox"</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3467,24 +3467,24 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>3810</t>
+          <t>3825</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>46065</t>
+          <t>59052</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>54588689</t>
+          <t>52792063</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>㊥墨衍枫迹☜</t>
+          <t>"Tramaine Dowlen"</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3494,24 +3494,24 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>3325</t>
+          <t>2800</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>35915</t>
+          <t>54842</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>52997727</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>larios</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3521,24 +3521,24 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>3776</t>
+          <t>2953</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>53368</t>
+          <t>35214</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>55499394</t>
+          <t>54085771</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Player-55499394</t>
+          <t>㊥Matthieu</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3548,24 +3548,24 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>3014</t>
+          <t>3810</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>34606</t>
+          <t>46065</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>54588689</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>㊥墨衍枫迹☜</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3575,24 +3575,24 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>3836</t>
+          <t>3325</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>58358</t>
+          <t>35915</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>55810157</t>
+          <t>54778421</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Beard</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3602,24 +3602,24 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>2823</t>
+          <t>3776</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>43081</t>
+          <t>53368</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>55499394</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Globalking</t>
+          <t>Player-55499394</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3629,24 +3629,24 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>3446</t>
+          <t>3014</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>44569</t>
+          <t>34606</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>55634661</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>Opalus</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3656,24 +3656,24 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>3386</t>
+          <t>3836</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>32416</t>
+          <t>58358</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>55810157</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>Beard</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3683,24 +3683,24 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>3923</t>
+          <t>2823</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>43125</t>
+          <t>43081</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>56732705</t>
+          <t>56379103</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>时间温柔皆遗憾</t>
+          <t>Globalking</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3710,24 +3710,24 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>3444</t>
+          <t>3446</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>85321</t>
+          <t>44569</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>57556179</t>
+          <t>56585361</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>特战新生代英雄</t>
+          <t>"㊥ go策划我要ali"</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3737,24 +3737,24 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>2247</t>
+          <t>3386</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>60972</t>
+          <t>32416</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>58203298</t>
+          <t>56700848</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>权旨qua</t>
+          <t>工口漫画老师</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3764,24 +3764,24 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>2741</t>
+          <t>3923</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>64818</t>
+          <t>43125</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>58340439</t>
+          <t>56732705</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>70qilin</t>
+          <t>时间温柔皆遗憾</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -3791,105 +3791,105 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>2637</t>
+          <t>3444</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>5822</t>
+          <t>85321</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>22497</t>
+          <t>57556179</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>xixihahagggᶻᵍˣ</t>
+          <t>特战新生代英雄</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>6015</t>
+          <t>2247</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>70042</t>
+          <t>60972</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>41463618</t>
+          <t>58203298</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>qi ye</t>
+          <t>权旨qua</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>2534</t>
+          <t>2741</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>58437</t>
+          <t>64818</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>41849539</t>
+          <t>58340439</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>三号馆馆主</t>
+          <t>70qilin</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>2820</t>
+          <t>2637</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>64031</t>
+          <t>5822</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>22497</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>xixihahagggᶻᵍˣ</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3899,24 +3899,24 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>2657</t>
+          <t>6015</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>31493</t>
+          <t>70042</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>41463618</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>qi ye</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -3926,24 +3926,24 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>3966</t>
+          <t>2534</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>58437</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>51816877</t>
+          <t>41849539</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>且行且珍惜</t>
+          <t>三号馆馆主</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3953,24 +3953,24 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2820</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>52742</t>
+          <t>64031</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>55210350</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>一个过客而已</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3980,24 +3980,24 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>3040</t>
+          <t>2657</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>56128</t>
+          <t>31493</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4007,24 +4007,24 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>2901</t>
+          <t>3966</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>62067</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>57219176</t>
+          <t>51816877</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>青莲道人</t>
+          <t>且行且珍惜</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4034,24 +4034,24 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>2711</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>73051</t>
+          <t>52742</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>57722377</t>
+          <t>55210350</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>VI空白IV</t>
+          <t>一个过客而已</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4061,24 +4061,24 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>2492</t>
+          <t>3040</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>56128</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>57742603</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>地铁逃生老六与白嫖仔</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4088,24 +4088,24 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>1907</t>
+          <t>2901</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>62067</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>57809206</t>
+          <t>57219176</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>"king 1"</t>
+          <t>青莲道人</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4115,24 +4115,24 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2711</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>73051</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>57847993</t>
+          <t>57722377</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>龘梦心裘千仞</t>
+          <t>VI空白IV</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4142,24 +4142,24 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>1508</t>
+          <t>2492</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>91159</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>57867293</t>
+          <t>57742603</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Player-57867293</t>
+          <t>地铁逃生老六与白嫖仔</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4169,24 +4169,24 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>2164</t>
+          <t>1907</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>89342</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>57905163</t>
+          <t>57809206</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>ABC—57905163</t>
+          <t>"king 1"</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4196,7 +4196,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>2190</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4208,12 +4208,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>57908454</t>
+          <t>57847993</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Player-57908454</t>
+          <t>龘梦心裘千仞</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4223,24 +4223,24 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>1508</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>91159</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>58310362</t>
+          <t>57867293</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>不老实的老实人</t>
+          <t>Player-57867293</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4250,24 +4250,24 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>1531</t>
+          <t>2164</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>89342</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>58368224</t>
+          <t>57905163</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>战争雷霆杯</t>
+          <t>ABC—57905163</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4277,7 +4277,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>1400</t>
+          <t>2190</t>
         </is>
       </c>
     </row>
@@ -4289,12 +4289,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>58380905</t>
+          <t>57908454</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Player-58380905</t>
+          <t>Player-57908454</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4304,7 +4304,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>1648</t>
+          <t>1100</t>
         </is>
       </c>
     </row>
@@ -4316,12 +4316,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>58386875</t>
+          <t>58310362</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>ExquisiteAgreement33</t>
+          <t>不老实的老实人</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4331,7 +4331,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>1328</t>
+          <t>1531</t>
         </is>
       </c>
     </row>
@@ -4343,12 +4343,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>58415620</t>
+          <t>58368224</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>"el pepe"</t>
+          <t>战争雷霆杯</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4358,7 +4358,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>1685</t>
+          <t>1400</t>
         </is>
       </c>
     </row>
@@ -4370,12 +4370,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>58425274</t>
+          <t>58380905</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Player-58425274</t>
+          <t>Player-58380905</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -4385,7 +4385,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>1411</t>
+          <t>1648</t>
         </is>
       </c>
     </row>
@@ -4397,12 +4397,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>58437456</t>
+          <t>58386875</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>中国人不骗中国人</t>
+          <t>ExquisiteAgreement33</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -4412,7 +4412,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>1639</t>
+          <t>1328</t>
         </is>
       </c>
     </row>
@@ -4424,12 +4424,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>58479166</t>
+          <t>58415620</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>ريانRedSomebody264</t>
+          <t>"el pepe"</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -4439,7 +4439,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>1140</t>
+          <t>1685</t>
         </is>
       </c>
     </row>
@@ -4451,12 +4451,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>58494374</t>
+          <t>58425274</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Kirinfire</t>
+          <t>Player-58425274</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -4466,7 +4466,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>1259</t>
+          <t>1411</t>
         </is>
       </c>
     </row>
@@ -4478,12 +4478,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>58526469</t>
+          <t>58437456</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>ItaloFlausino</t>
+          <t>中国人不骗中国人</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -4493,7 +4493,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>1781</t>
+          <t>1639</t>
         </is>
       </c>
     </row>
@@ -4505,12 +4505,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>58479166</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>ريانRedSomebody264</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -4520,7 +4520,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>1346</t>
+          <t>1140</t>
         </is>
       </c>
     </row>
@@ -4532,12 +4532,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>58584744</t>
+          <t>58494374</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>ronaldo</t>
+          <t>Kirinfire</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -4547,34 +4547,34 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>1198</t>
+          <t>1259</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>10575</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>6010122</t>
+          <t>58526469</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>"Edward Peng"</t>
+          <t>ItaloFlausino</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>5347</t>
+          <t>1781</t>
         </is>
       </c>
     </row>
@@ -4586,22 +4586,22 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>8850180</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>30624300</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1346</t>
         </is>
       </c>
     </row>
@@ -4613,39 +4613,39 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>9195340</t>
+          <t>58584744</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Namllllllik</t>
+          <t>ronaldo</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1198</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>4025</t>
+          <t>10575</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>9913517</t>
+          <t>6010122</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>"Kenny Chan"</t>
+          <t>"Edward Peng"</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -4655,7 +4655,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>6220</t>
+          <t>5347</t>
         </is>
       </c>
     </row>
@@ -4667,12 +4667,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>12648101</t>
+          <t>8850180</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>"player 198827"</t>
+          <t>30624300</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -4689,17 +4689,17 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>57473</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>15755724</t>
+          <t>9195340</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>"Last Good"</t>
+          <t>Namllllllik</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -4709,24 +4709,24 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>2853</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4025</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>28624723</t>
+          <t>9913517</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>"Woody Shade"</t>
+          <t>"Kenny Chan"</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -4736,32 +4736,113 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6220</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>12648101</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>"player 198827"</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>57473</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>15755724</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>"Last Good"</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>2853</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>28624723</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>"Woody Shade"</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
           <t>52177</t>
         </is>
       </c>
-      <c r="B163" t="inlineStr">
+      <c r="B166" t="inlineStr">
         <is>
           <t>41848598</t>
         </is>
       </c>
-      <c r="C163" t="inlineStr">
+      <c r="C166" t="inlineStr">
         <is>
           <t>国家一级保护沙雕</t>
         </is>
       </c>
-      <c r="D163" t="inlineStr">
+      <c r="D166" t="inlineStr">
         <is>
           <t>Chinese</t>
         </is>
       </c>
-      <c r="E163" t="inlineStr">
+      <c r="E166" t="inlineStr">
         <is>
           <t>3065</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-05-05 12:48:20
</commit_message>
<xml_diff>
--- a/Season_Trophies/81.xlsx
+++ b/Season_Trophies/81.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -396,17 +396,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5019</t>
+          <t>20274</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>36417892</t>
+          <t>20</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"VEC Para Bellum"</t>
+          <t>春田花花幼稚园</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -416,24 +416,24 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>6263</t>
+          <t>4604</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1870</t>
+          <t>4979</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8737186</t>
+          <t>1820342</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"Lukas      vec"</t>
+          <t>摸鱼者三战</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -443,24 +443,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>6791</t>
+          <t>6101</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2217</t>
+          <t>2035</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>31910959</t>
+          <t>1951758</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>VEC◇BONKERS</t>
+          <t>我來找你了</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -470,24 +470,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>6725</t>
+          <t>6583</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>3334</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>11935881</t>
+          <t>3477306</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ODKRO</t>
+          <t>"MeGa Tsai"</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -497,24 +497,24 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>6666</t>
+          <t>6330</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2859</t>
+          <t>3396</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>41975808</t>
+          <t>3946814</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Christian</t>
+          <t>"小瑩 潘"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -524,24 +524,24 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>6596</t>
+          <t>6320</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3270</t>
+          <t>7369</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2128417</t>
+          <t>4229136</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Jungle</t>
+          <t>"totoro wu"</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -551,24 +551,24 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>6531</t>
+          <t>5732</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>9716</t>
+          <t>4868</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>55822728</t>
+          <t>5691528</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"VEC Lil Bonkers"</t>
+          <t>ABearBear</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -578,24 +578,24 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>5777</t>
+          <t>6111</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>12056</t>
+          <t>41011</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>44358234</t>
+          <t>6016757</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"⚔️⛨ Nots 2 ᵛᵉᶜ"</t>
+          <t>Xx邪罗罗xX</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -605,24 +605,24 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>5591</t>
+          <t>3534</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>16014</t>
+          <t>7349</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>51221321</t>
+          <t>6510348</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>pocket</t>
+          <t>Bonpoisson</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -632,24 +632,24 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5286</t>
+          <t>5738</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>19870</t>
+          <t>424</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>36081694</t>
+          <t>6940556</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"⚔️Nots Pickle"</t>
+          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -659,24 +659,24 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>5062</t>
+          <t>7186</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>5789</t>
+          <t>5210</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>41582471</t>
+          <t>7025661</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>HAWK</t>
+          <t>"F ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -686,24 +686,24 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>6158</t>
+          <t>6075</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>8398</t>
+          <t>54417</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>28106548</t>
+          <t>7587898</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>V.A.A.S.</t>
+          <t>藍精靈ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -713,24 +713,24 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>5889</t>
+          <t>2970</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>15184</t>
+          <t>285</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>26306753</t>
+          <t>8741713</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"Ky DAD Vec"</t>
+          <t xml:space="preserve">㊥大咖玩家ky </t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -740,24 +740,24 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>5337</t>
+          <t>7281</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>15216</t>
+          <t>4899</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>28910224</t>
+          <t>9541747</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>"CooKI ᵛᵉᶜ"</t>
+          <t>豹子头林冲</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -767,24 +767,24 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>5335</t>
+          <t>6108</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>16576</t>
+          <t>1220</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>20718434</t>
+          <t>11783968</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3von.</t>
+          <t>F---119</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -794,24 +794,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>5251</t>
+          <t>6840</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>17708</t>
+          <t>8012</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10605547</t>
+          <t>14424176</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Siebu</t>
+          <t>天才少年老纪</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -821,24 +821,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>5181</t>
+          <t>5630</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>18119</t>
+          <t>3216</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>53985519</t>
+          <t>16206490</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"inky33 VEC"</t>
+          <t>㊥Godcys</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -848,24 +848,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>5156</t>
+          <t>6351</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>19657</t>
+          <t>524</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>46233038</t>
+          <t>20199374</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Arumonk</t>
+          <t>RuanFan</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -875,24 +875,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>5074</t>
+          <t>7137</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19701</t>
+          <t>6531</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>17862851</t>
+          <t>20737010</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"Sam Vimes"</t>
+          <t>混着玩...</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -902,24 +902,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>5071</t>
+          <t>5881</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20169</t>
+          <t>2303</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>8560877</t>
+          <t>21345373</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>VECBeerdsman</t>
+          <t>林北不講武德</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -929,24 +929,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>5044</t>
+          <t>6525</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>22691</t>
+          <t>4191</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>50248005</t>
+          <t>21665473</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Zyvis</t>
+          <t>"Dog Gamedesiger"</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -956,24 +956,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>4906</t>
+          <t>6196</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>23530</t>
+          <t>6768</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>10383351</t>
+          <t>21735478</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>SirScottsalot</t>
+          <t>耀翔fly</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -983,24 +983,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>4860</t>
+          <t>5834</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>23819</t>
+          <t>72376</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>50990927</t>
+          <t>23687250</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>"jetlijp ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1010,24 +1010,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4842</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>26968</t>
+          <t>3692</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>57009371</t>
+          <t>24733875</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>:Zam:</t>
+          <t>Kikkik</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1037,24 +1037,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>4684</t>
+          <t>6268</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>27392</t>
+          <t>2430</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>57874742</t>
+          <t>25376635</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>BmorelkmeAlt</t>
+          <t>"sanchez ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1064,24 +1064,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>4665</t>
+          <t>6492</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>29119</t>
+          <t>2769</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>707187</t>
+          <t>26280580</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>"Pacem ᵛᵉᶜ"</t>
+          <t>꧁S.TIGRESS꧂ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1091,24 +1091,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>4591</t>
+          <t>6426</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>31456</t>
+          <t>983</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>43626377</t>
+          <t>26424998</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>"The Kurgan VEC"</t>
+          <t>"煙神在此 爾等跪拜 ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1118,24 +1118,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>4495</t>
+          <t>6924</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>30749</t>
+          <t>4273</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>36042504</t>
+          <t>26588375</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>"Daveypb24 ⱽᵉᶜ"</t>
+          <t>kusipao</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1145,24 +1145,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>4522</t>
+          <t>6182</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>32942</t>
+          <t>2994</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>52574194</t>
+          <t>27468237</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>whyme</t>
+          <t>佛系复仇者秀川</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1172,24 +1172,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>4426</t>
+          <t>6388</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>33431</t>
+          <t>465</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>58274638</t>
+          <t>27484940</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>"Slash Ϟ"</t>
+          <t>"Zephyr ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1199,24 +1199,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4403</t>
+          <t>7167</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>35525</t>
+          <t>38845</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>54791976</t>
+          <t>28387448</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Rajman</t>
+          <t>☜⊙‖⊙☞</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4304</t>
+          <t>3632</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>38004</t>
+          <t>1880</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>57252217</t>
+          <t>29211638</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>DaJenius</t>
+          <t>"㊥ PhononDisperse"</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1253,24 +1253,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>4186</t>
+          <t>6623</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>40136</t>
+          <t>7894</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>54049077</t>
+          <t>29729468</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Wiedźmin</t>
+          <t>"风神舞动 WDᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1280,24 +1280,24 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4076</t>
+          <t>5648</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>41889</t>
+          <t>12555</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>41227593</t>
+          <t>29861826</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>"Arly Cleve OH-D"</t>
+          <t>★★★Eric★★★</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1307,24 +1307,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>3992</t>
+          <t>5194</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>51470</t>
+          <t>55810</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>58192944</t>
+          <t>30129740</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ScottieV༙྇e༙྇c༙྇</t>
+          <t>JohnyWS</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1334,24 +1334,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>3051</t>
+          <t>2915</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>4173</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>51052414</t>
+          <t>30411791</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Higoramp</t>
+          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1361,24 +1361,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6198</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>24891</t>
+          <t>7608</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>46302201</t>
+          <t>31217211</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Matty</t>
+          <t>解憂雜貨鋪㊥</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1388,24 +1388,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>4785</t>
+          <t>5695</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>27033</t>
+          <t>471</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>55603449</t>
+          <t>31267627</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>GameofThrones</t>
+          <t>"㊥ Martin"</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1415,24 +1415,24 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>4681</t>
+          <t>7164</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>29045</t>
+          <t>4466</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>24665950</t>
+          <t>32478707</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Triple-R</t>
+          <t>"Bt So"</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1442,24 +1442,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>4595</t>
+          <t>6157</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>29187</t>
+          <t>520</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>46477117</t>
+          <t>32613475</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>"Mama šč ⱽᵉᶜ"</t>
+          <t>"李 无 善 德"</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1469,24 +1469,24 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>4589</t>
+          <t>7138</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>34063</t>
+          <t>5754</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>34100839</t>
+          <t>33656016</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>nti3nn.xzyc</t>
+          <t>㊥☆梅海听雪☆</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1496,24 +1496,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>6021</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>40206</t>
+          <t>49144</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>57582503</t>
+          <t>35384730</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Revolutionize</t>
+          <t>"king of war £"</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1523,24 +1523,24 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>4072</t>
+          <t>3205</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>50594</t>
+          <t>6894</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>56139551</t>
+          <t>43800641</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>madani911</t>
+          <t>㊥蛋蛋大</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1550,24 +1550,24 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>3113</t>
+          <t>5813</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>51090</t>
+          <t>4111</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>58404624</t>
+          <t>44955827</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Skyler</t>
+          <t>丶小阿狸丿</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1577,24 +1577,24 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>3076</t>
+          <t>6207</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>57835</t>
+          <t>10530</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>54958241</t>
+          <t>45967307</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>clgray1976</t>
+          <t>Ricky</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1604,24 +1604,24 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2764</t>
+          <t>5351</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>76711</t>
+          <t>3122</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>59259842</t>
+          <t>46422609</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Supernova</t>
+          <t>㊥林天大大神</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1631,24 +1631,24 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2258</t>
+          <t>6366</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>82976</t>
+          <t>4509</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>57931192</t>
+          <t>47758619</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Killua</t>
+          <t>"㊥ Moon ㊥"</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1658,24 +1658,24 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2088</t>
+          <t>6152</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>120077</t>
+          <t>5504</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4998335</t>
+          <t>49553719</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>AHA...</t>
+          <t>"Oreo Captain Sir"</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1685,78 +1685,78 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1317</t>
+          <t>6046</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>54618</t>
+          <t>18691</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>29565</t>
+          <t>54189845</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>"aK.j Zhong ㊥"</t>
+          <t>"going down ®"</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2962</t>
+          <t>4684</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>44737</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>68132</t>
+          <t>57484853</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>"㊖TW9 百媚生"</t>
+          <t>"vector to islam"</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>3380</t>
+          <t>1997</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>27658</t>
+          <t>54618</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>1550355</t>
+          <t>29565</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>"皓茵 世界"</t>
+          <t>"aK.j Zhong ㊥"</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1766,24 +1766,24 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>4150</t>
+          <t>2962</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>7057</t>
+          <t>44737</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>4493731</t>
+          <t>68132</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Player-1527362</t>
+          <t>"㊖TW9 百媚生"</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1793,24 +1793,24 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>5784</t>
+          <t>3380</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>21025</t>
+          <t>27658</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>4756174</t>
+          <t>1550355</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>純希です</t>
+          <t>"皓茵 世界"</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1820,24 +1820,24 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>4567</t>
+          <t>4150</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>19494</t>
+          <t>7057</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>6809364</t>
+          <t>4493731</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>"Scorp IP"</t>
+          <t>Player-1527362</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1847,24 +1847,24 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>4640</t>
+          <t>5784</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>10360</t>
+          <t>21025</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7852598</t>
+          <t>4756174</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>seiji</t>
+          <t>純希です</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1874,24 +1874,24 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>5366</t>
+          <t>4567</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>17129</t>
+          <t>19494</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8057001</t>
+          <t>6809364</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>㊥兵者诡道也</t>
+          <t>"Scorp IP"</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1901,24 +1901,24 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>4781</t>
+          <t>4640</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>11028</t>
+          <t>10360</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>11582001</t>
+          <t>7852598</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>iMinatoX4</t>
+          <t>seiji</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1928,24 +1928,24 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>5311</t>
+          <t>5366</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>7359</t>
+          <t>17129</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>12639656</t>
+          <t>8057001</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>"wu huang"</t>
+          <t>㊥兵者诡道也</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1955,24 +1955,24 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>5735</t>
+          <t>4781</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>7428</t>
+          <t>11028</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>13738844</t>
+          <t>11582001</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>"Chen Hao"</t>
+          <t>iMinatoX4</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>5722</t>
+          <t>5311</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>32761</t>
+          <t>7359</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>14110169</t>
+          <t>12639656</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>"Pasiony CANQ"</t>
+          <t>"wu huang"</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,24 +2009,24 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>3910</t>
+          <t>5735</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>42232</t>
+          <t>7428</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>22161051</t>
+          <t>13738844</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Botz5</t>
+          <t>"Chen Hao"</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2036,24 +2036,24 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>3481</t>
+          <t>5722</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>10959</t>
+          <t>32761</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>22885399</t>
+          <t>14110169</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>余文琪</t>
+          <t>"Pasiony CANQ"</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2063,24 +2063,24 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>5316</t>
+          <t>3910</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>17046</t>
+          <t>42232</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>25435189</t>
+          <t>22161051</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Jose</t>
+          <t>Botz5</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2090,24 +2090,24 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>4787</t>
+          <t>3481</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6983</t>
+          <t>10959</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>28749280</t>
+          <t>22885399</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>㊥老船⛵⛵</t>
+          <t>余文琪</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2117,24 +2117,24 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>5795</t>
+          <t>5316</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>19000</t>
+          <t>17046</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>31495601</t>
+          <t>25435189</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>陈晓军</t>
+          <t>Jose</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>4666</t>
+          <t>4787</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>21345</t>
+          <t>6983</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>32316256</t>
+          <t>28749280</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>"秋の風 .."</t>
+          <t>㊥老船⛵⛵</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2171,24 +2171,24 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>4553</t>
+          <t>5795</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>22823</t>
+          <t>19000</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>37861953</t>
+          <t>31495601</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>"Durex ๑• . •๑"</t>
+          <t>陈晓军</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2198,24 +2198,24 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>4475</t>
+          <t>4666</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>25043</t>
+          <t>21345</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>38561634</t>
+          <t>32316256</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>"Ambrose PT"</t>
+          <t>"秋の風 .."</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2225,24 +2225,24 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>4311</t>
+          <t>4553</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>5950</t>
+          <t>22823</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>38711610</t>
+          <t>37861953</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>心灵有为</t>
+          <t>"Durex ๑• . •๑"</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2252,24 +2252,24 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>6001</t>
+          <t>4475</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>19776</t>
+          <t>25043</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>38809086</t>
+          <t>38561634</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Kouenᶻᵍˣ</t>
+          <t>"Ambrose PT"</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2279,24 +2279,24 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>4628</t>
+          <t>4311</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>22387</t>
+          <t>5950</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>38893233</t>
+          <t>38711610</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>"快乐 二哈"</t>
+          <t>心灵有为</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2306,24 +2306,24 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>4508</t>
+          <t>6001</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>31645</t>
+          <t>19776</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>38995116</t>
+          <t>38809086</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>"Ramesh Pavai Nam"</t>
+          <t>Kouenᶻᵍˣ</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2333,24 +2333,24 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>3959</t>
+          <t>4628</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>13559</t>
+          <t>22387</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>42434117</t>
+          <t>38893233</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>㊥有双飞鸟</t>
+          <t>"快乐 二哈"</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2360,24 +2360,24 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>5084</t>
+          <t>4508</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7178</t>
+          <t>31645</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>43812707</t>
+          <t>38995116</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>bbtt</t>
+          <t>"Ramesh Pavai Nam"</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2387,24 +2387,24 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>5763</t>
+          <t>3959</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>38496</t>
+          <t>13559</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>45070827</t>
+          <t>42434117</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>㊥山东老灶丿</t>
+          <t>㊥有双飞鸟</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2414,24 +2414,24 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>3648</t>
+          <t>5084</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>10090</t>
+          <t>7178</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>47131129</t>
+          <t>43812707</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>NAM</t>
+          <t>bbtt</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2441,24 +2441,24 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>5392</t>
+          <t>5763</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>21538</t>
+          <t>38496</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>47146736</t>
+          <t>45070827</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>"HK 品瑜"</t>
+          <t>㊥山东老灶丿</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2468,24 +2468,24 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>4545</t>
+          <t>3648</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>13976</t>
+          <t>10090</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>49710892</t>
+          <t>47131129</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>MMMMMMM</t>
+          <t>NAM</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2495,24 +2495,24 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>5042</t>
+          <t>5392</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>11960</t>
+          <t>21538</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>53060417</t>
+          <t>47146736</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>㊥老纳信耶稣</t>
+          <t>"HK 品瑜"</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2522,24 +2522,24 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>5240</t>
+          <t>4545</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>15232</t>
+          <t>13976</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>53520939</t>
+          <t>49710892</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>㊥虎哥tiger</t>
+          <t>MMMMMMM</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2549,24 +2549,24 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>4926</t>
+          <t>5042</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>15112</t>
+          <t>11960</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>54698813</t>
+          <t>53060417</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>閃亮唐老鴨</t>
+          <t>㊥老纳信耶稣</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2576,24 +2576,24 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>4938</t>
+          <t>5240</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>17132</t>
+          <t>15232</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>54915122</t>
+          <t>53520939</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>平胸救世界</t>
+          <t>㊥虎哥tiger</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2603,24 +2603,24 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>4781</t>
+          <t>4926</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>31018</t>
+          <t>15112</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>55769051</t>
+          <t>54698813</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>㊥叮叮当.</t>
+          <t>閃亮唐老鴨</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2630,24 +2630,24 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>3987</t>
+          <t>4938</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>33682</t>
+          <t>17132</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>55860890</t>
+          <t>54915122</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>㊥Ethan</t>
+          <t>平胸救世界</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2657,24 +2657,24 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>3873</t>
+          <t>4781</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>12260</t>
+          <t>31018</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>56133764</t>
+          <t>55769051</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>ustcarter</t>
+          <t>㊥叮叮当.</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2684,24 +2684,24 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>5219</t>
+          <t>3987</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>51526</t>
+          <t>33682</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>56500325</t>
+          <t>55860890</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>haruharuyukizg9735</t>
+          <t>㊥Ethan</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2711,24 +2711,24 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>3096</t>
+          <t>3873</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>40758</t>
+          <t>12260</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>56573048</t>
+          <t>56133764</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Xiaotian</t>
+          <t>ustcarter</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2738,24 +2738,24 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>3545</t>
+          <t>5219</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>93490</t>
+          <t>51526</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>57837683</t>
+          <t>56500325</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>我的世界只有你</t>
+          <t>haruharuyukizg9735</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2765,78 +2765,78 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2121</t>
+          <t>3096</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>57695</t>
+          <t>40758</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>1222440</t>
+          <t>56573048</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>"Sneaky Ninja Panda"</t>
+          <t>Xiaotian</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>2845</t>
+          <t>3545</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>48591</t>
+          <t>93490</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>57837683</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>我的世界只有你</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>3228</t>
+          <t>2121</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>75014</t>
+          <t>57695</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>5367482</t>
+          <t>1222440</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Ігор</t>
+          <t>"Sneaky Ninja Panda"</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2846,24 +2846,24 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>2459</t>
+          <t>2845</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>5428</t>
+          <t>48591</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>7857221</t>
+          <t>3391765</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Disparaître</t>
+          <t>马er</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2873,24 +2873,24 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>6055</t>
+          <t>3228</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>63090</t>
+          <t>75014</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>9718882</t>
+          <t>5367482</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>小霸王2021</t>
+          <t>Ігор</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2900,24 +2900,24 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>2681</t>
+          <t>2459</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>44682</t>
+          <t>5428</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>7857221</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>Disparaître</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2927,24 +2927,24 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>3383</t>
+          <t>6055</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>39181</t>
+          <t>63090</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>18082891</t>
+          <t>9718882</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>小霸王2021</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2954,24 +2954,24 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>3616</t>
+          <t>2681</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>20050</t>
+          <t>44682</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>25163202</t>
+          <t>11645391</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>"sam yang"</t>
+          <t>"omar omar"</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2981,24 +2981,24 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>4614</t>
+          <t>3383</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>26837</t>
+          <t>39181</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>25479797</t>
+          <t>18082891</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>"Mohamed Alnaqbi"</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3008,24 +3008,24 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>4197</t>
+          <t>3616</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>30580</t>
+          <t>20050</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>28855852</t>
+          <t>25163202</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>tiger</t>
+          <t>"sam yang"</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3035,24 +3035,24 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>4006</t>
+          <t>4614</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>18919</t>
+          <t>26837</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>25479797</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>"Mohamed Alnaqbi"</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3062,24 +3062,24 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>4671</t>
+          <t>4197</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>29874</t>
+          <t>30580</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>37069173</t>
+          <t>28855852</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>詹toniii</t>
+          <t>tiger</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3089,24 +3089,24 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>4038</t>
+          <t>4006</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>53460</t>
+          <t>18919</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>38994054</t>
+          <t>31134300</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>chengnan</t>
+          <t>McMaX</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3116,24 +3116,24 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>3011</t>
+          <t>4671</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>7503</t>
+          <t>29874</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>44378757</t>
+          <t>37069173</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
+          <t>詹toniii</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3143,24 +3143,24 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>5710</t>
+          <t>4038</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>28150</t>
+          <t>53460</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>44708798</t>
+          <t>38994054</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>"㊥ mythgod"</t>
+          <t>chengnan</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3170,24 +3170,24 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>4124</t>
+          <t>3011</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>38060</t>
+          <t>7503</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>46289694</t>
+          <t>44378757</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>㊥Vincent</t>
+          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3197,24 +3197,24 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>3670</t>
+          <t>5710</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>57118</t>
+          <t>28150</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>47227626</t>
+          <t>44708798</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Player-47227626</t>
+          <t>"㊥ mythgod"</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3224,24 +3224,24 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>2865</t>
+          <t>4124</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>29363</t>
+          <t>38060</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>46289694</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>㊥Vincent</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3251,24 +3251,24 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>4064</t>
+          <t>3670</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>37595</t>
+          <t>57118</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>47227626</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>Player-47227626</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3278,24 +3278,24 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>3693</t>
+          <t>2865</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>30760</t>
+          <t>29363</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3305,24 +3305,24 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>3998</t>
+          <t>4064</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>34858</t>
+          <t>37595</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>51841127</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>"Muhammad Shox"</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3332,24 +3332,24 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>3825</t>
+          <t>3693</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>59052</t>
+          <t>30760</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>52792063</t>
+          <t>48634530</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>"Tramaine Dowlen"</t>
+          <t>leezhenrui</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3359,24 +3359,24 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>2800</t>
+          <t>3998</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>54842</t>
+          <t>34858</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>51841127</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>"Muhammad Shox"</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3386,24 +3386,24 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>2953</t>
+          <t>3825</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>35214</t>
+          <t>59052</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>52792063</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>"Tramaine Dowlen"</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3413,24 +3413,24 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>3810</t>
+          <t>2800</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>46065</t>
+          <t>54842</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>54588689</t>
+          <t>52997727</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>㊥墨衍枫迹☜</t>
+          <t>larios</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3440,24 +3440,24 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>3325</t>
+          <t>2953</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>35915</t>
+          <t>35214</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>54085771</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>㊥Matthieu</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3467,24 +3467,24 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>3776</t>
+          <t>3810</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>53368</t>
+          <t>46065</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>55499394</t>
+          <t>54588689</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Player-55499394</t>
+          <t>㊥墨衍枫迹☜</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3494,24 +3494,24 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>3014</t>
+          <t>3325</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>34606</t>
+          <t>35915</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>54778421</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3521,24 +3521,24 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>3836</t>
+          <t>3776</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>58358</t>
+          <t>53368</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>55810157</t>
+          <t>55499394</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Beard</t>
+          <t>Player-55499394</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3548,24 +3548,24 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>2823</t>
+          <t>3014</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>43081</t>
+          <t>34606</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>55634661</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Globalking</t>
+          <t>Opalus</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3575,24 +3575,24 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>3446</t>
+          <t>3836</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>44569</t>
+          <t>58358</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>55810157</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>Beard</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3602,24 +3602,24 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>3386</t>
+          <t>2823</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>32416</t>
+          <t>43081</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>56379103</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>Globalking</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3629,24 +3629,24 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>3923</t>
+          <t>3446</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>43125</t>
+          <t>44569</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>56732705</t>
+          <t>56585361</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>时间温柔皆遗憾</t>
+          <t>"㊥ go策划我要ali"</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3656,24 +3656,24 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>3444</t>
+          <t>3386</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>85321</t>
+          <t>32416</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>57556179</t>
+          <t>56700848</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>特战新生代英雄</t>
+          <t>工口漫画老师</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3683,24 +3683,24 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>2247</t>
+          <t>3923</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>60972</t>
+          <t>43125</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>58203298</t>
+          <t>56732705</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>权旨qua</t>
+          <t>时间温柔皆遗憾</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3710,24 +3710,24 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>2741</t>
+          <t>3444</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>64818</t>
+          <t>85321</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>58340439</t>
+          <t>57556179</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>70qilin</t>
+          <t>特战新生代英雄</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3737,78 +3737,78 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>2637</t>
+          <t>2247</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>5822</t>
+          <t>60972</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>22497</t>
+          <t>58203298</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>xixihahagggᶻᵍˣ</t>
+          <t>权旨qua</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>6015</t>
+          <t>2741</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>70042</t>
+          <t>64818</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>41463618</t>
+          <t>58340439</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>qi ye</t>
+          <t>70qilin</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>2534</t>
+          <t>2637</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>58437</t>
+          <t>5822</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>41849539</t>
+          <t>22497</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>三号馆馆主</t>
+          <t>xixihahagggᶻᵍˣ</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3818,24 +3818,24 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>2820</t>
+          <t>6015</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>64031</t>
+          <t>70042</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>41463618</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>qi ye</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -3845,24 +3845,24 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>2657</t>
+          <t>2534</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>31493</t>
+          <t>58437</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>41849539</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>三号馆馆主</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3872,24 +3872,24 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>3966</t>
+          <t>2820</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>64031</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>51816877</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>且行且珍惜</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3899,24 +3899,24 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2657</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>52742</t>
+          <t>31493</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>55210350</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>一个过客而已</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -3926,24 +3926,24 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>3040</t>
+          <t>3966</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>56128</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>51816877</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>且行且珍惜</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3953,24 +3953,24 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>2901</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>62067</t>
+          <t>52742</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>57219176</t>
+          <t>55210350</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>青莲道人</t>
+          <t>一个过客而已</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3980,24 +3980,24 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>2711</t>
+          <t>3040</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>73051</t>
+          <t>56128</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>57722377</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>VI空白IV</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4007,24 +4007,24 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>2492</t>
+          <t>2901</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>62067</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>57742603</t>
+          <t>57219176</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>地铁逃生老六与白嫖仔</t>
+          <t>青莲道人</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4034,24 +4034,24 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>1907</t>
+          <t>2711</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>73051</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>57809206</t>
+          <t>57722377</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>"king 1"</t>
+          <t>VI空白IV</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2492</t>
         </is>
       </c>
     </row>
@@ -4073,12 +4073,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>57847993</t>
+          <t>57742603</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>龘梦心裘千仞</t>
+          <t>地铁逃生老六与白嫖仔</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4088,24 +4088,24 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>1508</t>
+          <t>1907</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>91159</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>57867293</t>
+          <t>57809206</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Player-57867293</t>
+          <t>"king 1"</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4115,24 +4115,24 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>2164</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>89342</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>57905163</t>
+          <t>57847993</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>ABC—57905163</t>
+          <t>龘梦心裘千仞</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4142,24 +4142,24 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>2190</t>
+          <t>1508</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>91159</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>57908454</t>
+          <t>57867293</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Player-57908454</t>
+          <t>Player-57867293</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4169,24 +4169,24 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>2164</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>89342</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>58310362</t>
+          <t>57905163</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>不老实的老实人</t>
+          <t>ABC—57905163</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4196,7 +4196,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>1531</t>
+          <t>2190</t>
         </is>
       </c>
     </row>
@@ -4208,12 +4208,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>58368224</t>
+          <t>57908454</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>战争雷霆杯</t>
+          <t>Player-57908454</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4223,7 +4223,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>1400</t>
+          <t>1100</t>
         </is>
       </c>
     </row>
@@ -4235,12 +4235,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>58380905</t>
+          <t>58310362</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Player-58380905</t>
+          <t>不老实的老实人</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4250,7 +4250,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>1648</t>
+          <t>1531</t>
         </is>
       </c>
     </row>
@@ -4262,12 +4262,12 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>58386875</t>
+          <t>58368224</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>ExquisiteAgreement33</t>
+          <t>战争雷霆杯</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4277,7 +4277,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>1328</t>
+          <t>1400</t>
         </is>
       </c>
     </row>
@@ -4289,12 +4289,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>58415620</t>
+          <t>58380905</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>"el pepe"</t>
+          <t>Player-58380905</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4304,7 +4304,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>1685</t>
+          <t>1648</t>
         </is>
       </c>
     </row>
@@ -4316,12 +4316,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>58425274</t>
+          <t>58386875</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Player-58425274</t>
+          <t>ExquisiteAgreement33</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4331,7 +4331,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>1411</t>
+          <t>1328</t>
         </is>
       </c>
     </row>
@@ -4343,12 +4343,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>58437456</t>
+          <t>58415620</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>中国人不骗中国人</t>
+          <t>"el pepe"</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4358,7 +4358,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>1639</t>
+          <t>1685</t>
         </is>
       </c>
     </row>
@@ -4370,12 +4370,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>58479166</t>
+          <t>58425274</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>ريانRedSomebody264</t>
+          <t>Player-58425274</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -4385,7 +4385,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>1140</t>
+          <t>1411</t>
         </is>
       </c>
     </row>
@@ -4397,12 +4397,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>58494374</t>
+          <t>58437456</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Kirinfire</t>
+          <t>中国人不骗中国人</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -4412,7 +4412,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>1259</t>
+          <t>1639</t>
         </is>
       </c>
     </row>
@@ -4424,12 +4424,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>58526469</t>
+          <t>58479166</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>ItaloFlausino</t>
+          <t>ريانRedSomebody264</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -4439,7 +4439,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>1781</t>
+          <t>1140</t>
         </is>
       </c>
     </row>
@@ -4451,12 +4451,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>58494374</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>Kirinfire</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -4466,7 +4466,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>1346</t>
+          <t>1259</t>
         </is>
       </c>
     </row>
@@ -4478,12 +4478,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>58584744</t>
+          <t>58526469</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>ronaldo</t>
+          <t>ItaloFlausino</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -4493,34 +4493,34 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>1198</t>
+          <t>1781</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10575</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>6010122</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>"Edward Peng"</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>5347</t>
+          <t>1346</t>
         </is>
       </c>
     </row>
@@ -4532,39 +4532,39 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>8850180</t>
+          <t>58584744</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>30624300</t>
+          <t>ronaldo</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1198</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>10575</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>9195340</t>
+          <t>6010122</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Namllllllik</t>
+          <t>"Edward Peng"</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -4574,24 +4574,24 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5347</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>4025</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>9913517</t>
+          <t>8850180</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>"Kenny Chan"</t>
+          <t>30624300</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -4601,7 +4601,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>6220</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4613,12 +4613,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>12648101</t>
+          <t>9195340</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>"player 198827"</t>
+          <t>Namllllllik</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -4635,17 +4635,17 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>57473</t>
+          <t>4025</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>15755724</t>
+          <t>9913517</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>"Last Good"</t>
+          <t>"Kenny Chan"</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -4655,7 +4655,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>2853</t>
+          <t>6220</t>
         </is>
       </c>
     </row>
@@ -4667,12 +4667,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>28624723</t>
+          <t>12648101</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>"Woody Shade"</t>
+          <t>"player 198827"</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -4689,25 +4689,79 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
+          <t>57473</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>15755724</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>"Last Good"</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>2853</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>28624723</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>"Woody Shade"</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
           <t>52177</t>
         </is>
       </c>
-      <c r="B161" t="inlineStr">
+      <c r="B163" t="inlineStr">
         <is>
           <t>41848598</t>
         </is>
       </c>
-      <c r="C161" t="inlineStr">
+      <c r="C163" t="inlineStr">
         <is>
           <t>国家一级保护沙雕</t>
         </is>
       </c>
-      <c r="D161" t="inlineStr">
+      <c r="D163" t="inlineStr">
         <is>
           <t>Chinese</t>
         </is>
       </c>
-      <c r="E161" t="inlineStr">
+      <c r="E163" t="inlineStr">
         <is>
           <t>3065</t>
         </is>

</xml_diff>